<commit_message>
Appended the excel file
</commit_message>
<xml_diff>
--- a/CUDA data.xlsx
+++ b/CUDA data.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDANG\PES\SEM 6\HPC\CUDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7F802D50-7A7D-4E3C-B72F-BA14C930E8D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A09D0B06-26CC-4212-B747-01AD217474F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{629A8BFC-5F47-4E03-9532-2016D6483248}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,23 +34,34 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>GPU time</t>
+    <t>Iterations</t>
   </si>
   <si>
-    <t>CPU time</t>
+    <t>GPU time(ms)</t>
   </si>
   <si>
-    <t>Iterations</t>
+    <t>CPU time(ms)</t>
+  </si>
+  <si>
+    <t>Performace improved</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -78,12 +89,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -181,11 +195,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
+              <c:f>Data!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>GPU time</c:v>
+                  <c:v>GPU time(ms)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -210,7 +224,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$6</c:f>
+              <c:f>Data!$A$2:$A$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -234,7 +248,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$6</c:f>
+              <c:f>Data!$B$2:$B$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -268,11 +282,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
+              <c:f>Data!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>CPU time</c:v>
+                  <c:v>CPU time(ms)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -297,7 +311,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$6</c:f>
+              <c:f>Data!$A$2:$A$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -321,7 +335,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$6</c:f>
+              <c:f>Data!$C$2:$C$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1284,16 +1298,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>44450</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>463550</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>165100</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1621,38 +1635,42 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11.1796875" customWidth="1"/>
-    <col min="2" max="2" width="10.54296875" customWidth="1"/>
-    <col min="3" max="3" width="10.7265625" customWidth="1"/>
+    <col min="2" max="2" width="13.90625" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="22.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>10</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>3.6492300000000002</v>
       </c>
       <c r="C2" s="1">
         <v>108.44</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <f t="shared" ref="D2:D5" si="0">C2/B2</f>
         <v>29.715857865905956</v>
       </c>
@@ -1667,7 +1685,7 @@
       <c r="C3" s="1">
         <v>1535.22</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
         <f t="shared" si="0"/>
         <v>37.907134655983413</v>
       </c>
@@ -1682,7 +1700,7 @@
       <c r="C4" s="1">
         <v>5120.07</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <f t="shared" si="0"/>
         <v>22.980359242735702</v>
       </c>
@@ -1697,7 +1715,7 @@
       <c r="C5" s="1">
         <v>12326.3</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <f t="shared" si="0"/>
         <v>36.439665825119874</v>
       </c>
@@ -1712,7 +1730,7 @@
       <c r="C6" s="1">
         <v>53306.3</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="2">
         <f>C6/B6</f>
         <v>28.98719928655327</v>
       </c>

</xml_diff>